<commit_message>
PWC 395047 units 1-9 run on 2/1/25
</commit_message>
<xml_diff>
--- a/$Calibrtation/CAL_Level_RnR_241105.xlsx
+++ b/$Calibrtation/CAL_Level_RnR_241105.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AllenProjects\PWC-OLS\$Calibrtation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4DA945-A142-4FB9-B9D5-F061380E2047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734210EB-687F-47D2-9527-62A4471710E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18820" windowHeight="11280" xr2:uid="{E8277EBF-8E94-4486-9664-CBE43E0BB732}"/>
+    <workbookView xWindow="190" yWindow="1850" windowWidth="17550" windowHeight="11280" xr2:uid="{E8277EBF-8E94-4486-9664-CBE43E0BB732}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="54">
   <si>
     <t>Index</t>
   </si>
@@ -69,18 +69,148 @@
   </si>
   <si>
     <t>rob</t>
+  </si>
+  <si>
+    <t>CHA</t>
+  </si>
+  <si>
+    <t>CHB</t>
+  </si>
+  <si>
+    <t>VOM</t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>LV-Volts</t>
+  </si>
+  <si>
+    <t>LV-Rcalc</t>
+  </si>
+  <si>
+    <t>SUMMARY OUTPUT</t>
+  </si>
+  <si>
+    <t>Regression Statistics</t>
+  </si>
+  <si>
+    <t>Multiple R</t>
+  </si>
+  <si>
+    <t>R Square</t>
+  </si>
+  <si>
+    <t>Adjusted R Square</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>ANOVA</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Significance F</t>
+  </si>
+  <si>
+    <t>Coefficients</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Lower 95%</t>
+  </si>
+  <si>
+    <t>Upper 95%</t>
+  </si>
+  <si>
+    <t>RESIDUAL OUTPUT</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Residuals</t>
+  </si>
+  <si>
+    <t>Predicted VOM</t>
+  </si>
+  <si>
+    <t>C HB</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Cal</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>LV Leevel PV</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Lower 95.0%</t>
+  </si>
+  <si>
+    <t>Upper 95.0%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm;@"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +224,14 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -103,7 +241,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -126,17 +264,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +333,947 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>VOM  Residual Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$85:$D$89</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>499.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>899.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1098.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299.70999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$115:$C$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.25949708939953098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.861603670860859E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0016235604268786</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.69772725632856236</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2168220094254139E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2751-41FA-AAF4-A980CA2549BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="869746960"/>
+        <c:axId val="1196568815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="869746960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>VOM</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1196568815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1196568815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="869746960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>VOM  Residual Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$85:$D$89</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>499.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>899.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1098.0999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>299.70999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$115:$C$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.25949708939953098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.861603670860859E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0016235604268786</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.69772725632856236</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2168220094254139E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B60E-4E1C-A13D-43B48858ADB1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="982071743"/>
+        <c:axId val="982072223"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="982071743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>VOM</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="982072223"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="982072223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="982071743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LV-Volts  Residual Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$85:$B$89</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.8555999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5786</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1281999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$115:$C$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-0.25949708939953098</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.861603670860859E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0016235604268786</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.69772725632856236</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2168220094254139E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4BC4-49D9-BBC8-DDBD23019442}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1047009039"/>
+        <c:axId val="1047009999"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1047009039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>LV-Volts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1047009999"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1047009999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1047009039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LV-Volts  Residual Plot</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$85:$F$89</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.8641999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.58230000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1459000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2885999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7212000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$115:$L$119</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-9.4639267302909502E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.10419988676474645</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22029594005186937</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.18879526397495283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2163137418206134E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4D28-457F-97E9-735DF9C48073}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="980929759"/>
+        <c:axId val="980926399"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="980929759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>LV-Volts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="980926399"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="980926399"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Residuals</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="980929759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E854A55-B724-F18C-390C-D4F3B8284AF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DF0C5D5-BE66-5522-1296-9A18CAB87EB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B814C6-2ED9-5F99-3613-64B9912DD4FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA39268-9515-20A3-918B-04538EDE44BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -471,16 +1593,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B140EEA4-24B7-4406-9362-3B8CBBDD5496}">
-  <dimension ref="A2:G80"/>
+  <dimension ref="A2:P150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="4" width="13.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="13.54296875" style="3" customWidth="1"/>
     <col min="5" max="9" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1522,8 +2645,1177 @@
         <v>2</v>
       </c>
     </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>15</v>
+      </c>
+      <c r="B84" t="s">
+        <v>16</v>
+      </c>
+      <c r="C84" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>17</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K84" s="3"/>
+      <c r="L84" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M84" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N84" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>5.8010000000000002</v>
+      </c>
+      <c r="B85" s="6">
+        <v>2.8555999999999999</v>
+      </c>
+      <c r="C85">
+        <f t="shared" ref="C85:C88" si="0">B85/E85*1000</f>
+        <v>500.63113604488075</v>
+      </c>
+      <c r="D85" s="3">
+        <v>499.5</v>
+      </c>
+      <c r="E85" s="3">
+        <v>5.7039999999999997</v>
+      </c>
+      <c r="F85" s="6">
+        <v>2.8641999999999999</v>
+      </c>
+      <c r="G85">
+        <f t="shared" ref="G85:G88" si="1">F85/I85*1000</f>
+        <v>501.34780325573246</v>
+      </c>
+      <c r="H85" s="3">
+        <v>500.1</v>
+      </c>
+      <c r="I85" s="3">
+        <v>5.7130000000000001</v>
+      </c>
+      <c r="L85" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M85" s="10">
+        <v>-1.2696078443133274</v>
+      </c>
+      <c r="N85" s="10">
+        <v>-1.4679046096952106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>7.9039999999999999</v>
+      </c>
+      <c r="B86" s="6">
+        <v>0.5786</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="0"/>
+        <v>101.41980718667836</v>
+      </c>
+      <c r="D86" s="3">
+        <v>100.2</v>
+      </c>
+      <c r="E86" s="3">
+        <v>5.7050000000000001</v>
+      </c>
+      <c r="F86" s="6">
+        <v>0.58230000000000004</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="1"/>
+        <v>101.92543322247506</v>
+      </c>
+      <c r="H86" s="3">
+        <v>100.4</v>
+      </c>
+      <c r="I86" s="3">
+        <v>5.7130000000000001</v>
+      </c>
+      <c r="L86" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M86" s="10">
+        <v>175.45493239029025</v>
+      </c>
+      <c r="N86" s="10">
+        <v>175.11953373941259</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>4.0579999999999998</v>
+      </c>
+      <c r="B87" s="6">
+        <v>5.1281999999999996</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="0"/>
+        <v>899.36864258155026</v>
+      </c>
+      <c r="D87" s="3">
+        <v>899.5</v>
+      </c>
+      <c r="E87" s="3">
+        <v>5.702</v>
+      </c>
+      <c r="F87" s="6">
+        <v>5.1459000000000001</v>
+      </c>
+      <c r="G87">
+        <f t="shared" si="1"/>
+        <v>900.89285714285711</v>
+      </c>
+      <c r="H87" s="3">
+        <v>899.9</v>
+      </c>
+      <c r="I87" s="3">
+        <v>5.7119999999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>2.71</v>
+      </c>
+      <c r="B88" s="6">
+        <v>6.2698</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="0"/>
+        <v>1099.3862879186393</v>
+      </c>
+      <c r="D88" s="3">
+        <v>1098.0999999999999</v>
+      </c>
+      <c r="E88" s="3">
+        <v>5.7030000000000003</v>
+      </c>
+      <c r="F88" s="6">
+        <v>6.2885999999999997</v>
+      </c>
+      <c r="G88">
+        <f t="shared" si="1"/>
+        <v>1101.1381544388021</v>
+      </c>
+      <c r="H88" s="3">
+        <v>1099.5999999999999</v>
+      </c>
+      <c r="I88" s="3">
+        <v>5.7110000000000003</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>6.7720000000000002</v>
+      </c>
+      <c r="B89" s="6">
+        <v>1.7154</v>
+      </c>
+      <c r="C89">
+        <f>B89/E89*1000</f>
+        <v>300.78905839032086</v>
+      </c>
+      <c r="D89" s="3">
+        <v>299.70999999999998</v>
+      </c>
+      <c r="E89" s="3">
+        <v>5.7030000000000003</v>
+      </c>
+      <c r="F89" s="6">
+        <v>1.7212000000000001</v>
+      </c>
+      <c r="G89">
+        <f>F89/I89*1000</f>
+        <v>301.22506125306262</v>
+      </c>
+      <c r="H89" s="3">
+        <v>300.02999999999997</v>
+      </c>
+      <c r="I89" s="3">
+        <v>5.7140000000000004</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91"/>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="J91" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B92"/>
+      <c r="C92"/>
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A93" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B93" s="9"/>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="J93" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K93" s="9"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>20</v>
+      </c>
+      <c r="B94">
+        <v>0.99999886272079019</v>
+      </c>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="J94" t="s">
+        <v>20</v>
+      </c>
+      <c r="K94">
+        <v>0.99999992586858166</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B95">
+        <v>0.9999977254428738</v>
+      </c>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="J95" t="s">
+        <v>21</v>
+      </c>
+      <c r="K95">
+        <v>0.99999985173716877</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96">
+        <v>0.99999696725716503</v>
+      </c>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="J96" t="s">
+        <v>22</v>
+      </c>
+      <c r="K96">
+        <v>0.99999980231622498</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97">
+        <v>0.72106243859228891</v>
+      </c>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="J97" t="s">
+        <v>23</v>
+      </c>
+      <c r="K97">
+        <v>0.18427508093790479</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="7">
+        <v>5</v>
+      </c>
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="J98" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K98" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B99"/>
+      <c r="C99"/>
+      <c r="D99"/>
+    </row>
+    <row r="100" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>25</v>
+      </c>
+      <c r="B100"/>
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="J100" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A101" s="8"/>
+      <c r="B101" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E101" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F101" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L101" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="M101" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N101" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O101" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>26</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>685755.28628687887</v>
+      </c>
+      <c r="D102">
+        <v>685755.28628687887</v>
+      </c>
+      <c r="E102">
+        <v>1318935.0761343678</v>
+      </c>
+      <c r="F102">
+        <v>1.4559096792981664E-9</v>
+      </c>
+      <c r="J102" t="s">
+        <v>26</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>687103.43884808361</v>
+      </c>
+      <c r="M102">
+        <v>687103.43884808361</v>
+      </c>
+      <c r="N102">
+        <v>20234333.367978163</v>
+      </c>
+      <c r="O102">
+        <v>2.4229101953981534E-11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>27</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+      <c r="C103">
+        <v>1.5597931210459752</v>
+      </c>
+      <c r="D103">
+        <v>0.51993104034865845</v>
+      </c>
+      <c r="J103" t="s">
+        <v>27</v>
+      </c>
+      <c r="K103">
+        <v>3</v>
+      </c>
+      <c r="L103">
+        <v>0.10187191636401409</v>
+      </c>
+      <c r="M103">
+        <v>3.3957305454671363E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B104" s="7">
+        <v>4</v>
+      </c>
+      <c r="C104" s="7">
+        <v>685756.84607999993</v>
+      </c>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="J104" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K104" s="7">
+        <v>4</v>
+      </c>
+      <c r="L104" s="7">
+        <v>687103.54071999993</v>
+      </c>
+      <c r="M104" s="7"/>
+      <c r="N104" s="7"/>
+      <c r="O104" s="7"/>
+    </row>
+    <row r="105" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B105"/>
+      <c r="C105"/>
+      <c r="D105"/>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A106" s="8"/>
+      <c r="B106" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J106" s="8"/>
+      <c r="K106" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L106" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M106" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="N106" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O106" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P106" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>29</v>
+      </c>
+      <c r="B107">
+        <v>-1.2696078443133274</v>
+      </c>
+      <c r="C107">
+        <v>0.59969282134230262</v>
+      </c>
+      <c r="D107">
+        <v>-2.1170969521888598</v>
+      </c>
+      <c r="E107">
+        <v>0.12452499338856744</v>
+      </c>
+      <c r="F107">
+        <v>-3.1780980478993017</v>
+      </c>
+      <c r="G107">
+        <v>0.63888235927264692</v>
+      </c>
+      <c r="J107" t="s">
+        <v>29</v>
+      </c>
+      <c r="K107">
+        <v>-1.4679046096952106</v>
+      </c>
+      <c r="L107">
+        <v>0.15330124870526513</v>
+      </c>
+      <c r="M107">
+        <v>-9.5752945399510985</v>
+      </c>
+      <c r="N107">
+        <v>2.4166826774566466E-3</v>
+      </c>
+      <c r="O107">
+        <v>-1.9557776022326605</v>
+      </c>
+      <c r="P107">
+        <v>-0.98003161715776066</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A108" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B108" s="7">
+        <v>175.45493239029025</v>
+      </c>
+      <c r="C108" s="7">
+        <v>0.15277555585857949</v>
+      </c>
+      <c r="D108" s="7">
+        <v>1148.4489871711185</v>
+      </c>
+      <c r="E108" s="7">
+        <v>1.4559096792981664E-9</v>
+      </c>
+      <c r="F108" s="7">
+        <v>174.96873238701045</v>
+      </c>
+      <c r="G108" s="7">
+        <v>175.94113239357006</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K108" s="7">
+        <v>175.11953373941259</v>
+      </c>
+      <c r="L108" s="7">
+        <v>3.893051436319004E-2</v>
+      </c>
+      <c r="M108" s="7">
+        <v>4498.2589262933889</v>
+      </c>
+      <c r="N108" s="7">
+        <v>2.4229101953981534E-11</v>
+      </c>
+      <c r="O108" s="7">
+        <v>174.99563946781467</v>
+      </c>
+      <c r="P108" s="7">
+        <v>175.24342801101051</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B109"/>
+      <c r="C109"/>
+      <c r="D109"/>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B110"/>
+      <c r="C110"/>
+      <c r="D110"/>
+    </row>
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B111"/>
+      <c r="C111"/>
+      <c r="D111"/>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>40</v>
+      </c>
+      <c r="B112"/>
+      <c r="C112"/>
+      <c r="D112"/>
+      <c r="J112" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B113"/>
+      <c r="C113"/>
+      <c r="D113"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A114" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D114"/>
+      <c r="J114" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K114" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L114" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>499.75949708939953</v>
+      </c>
+      <c r="C115">
+        <v>-0.25949708939953098</v>
+      </c>
+      <c r="D115"/>
+      <c r="J115">
+        <v>1</v>
+      </c>
+      <c r="K115">
+        <v>500.10946392673031</v>
+      </c>
+      <c r="L115">
+        <v>-9.4639267302909502E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>2</v>
+      </c>
+      <c r="B116">
+        <v>100.24861603670861</v>
+      </c>
+      <c r="C116">
+        <v>-4.861603670860859E-2</v>
+      </c>
+      <c r="D116"/>
+      <c r="J116">
+        <v>2</v>
+      </c>
+      <c r="K116">
+        <v>100.50419988676475</v>
+      </c>
+      <c r="L116">
+        <v>-0.10419988676474645</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>3</v>
+      </c>
+      <c r="B117">
+        <v>898.49837643957312</v>
+      </c>
+      <c r="C117">
+        <v>1.0016235604268786</v>
+      </c>
+      <c r="D117"/>
+      <c r="J117">
+        <v>3</v>
+      </c>
+      <c r="K117">
+        <v>899.67970405994811</v>
+      </c>
+      <c r="L117">
+        <v>0.22029594005186937</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>4</v>
+      </c>
+      <c r="B118">
+        <v>1098.7977272563285</v>
+      </c>
+      <c r="C118">
+        <v>-0.69772725632856236</v>
+      </c>
+      <c r="D118"/>
+      <c r="J118">
+        <v>4</v>
+      </c>
+      <c r="K118">
+        <v>1099.7887952639749</v>
+      </c>
+      <c r="L118">
+        <v>-0.18879526397495283</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="7">
+        <v>5</v>
+      </c>
+      <c r="B119" s="7">
+        <v>299.70578317799055</v>
+      </c>
+      <c r="C119" s="7">
+        <v>4.2168220094254139E-3</v>
+      </c>
+      <c r="D119"/>
+      <c r="J119" s="7">
+        <v>5</v>
+      </c>
+      <c r="K119" s="7">
+        <v>299.94783686258177</v>
+      </c>
+      <c r="L119" s="7">
+        <v>8.2163137418206134E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A120" s="3"/>
+      <c r="B120"/>
+      <c r="C120"/>
+      <c r="D120"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A121" s="3"/>
+      <c r="B121"/>
+      <c r="C121"/>
+      <c r="D121"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A122" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B122" s="5">
+        <v>45689.458333333336</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A123" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A124" s="1">
+        <v>1</v>
+      </c>
+      <c r="B124" s="2">
+        <v>4.3879999999999999</v>
+      </c>
+      <c r="C124" s="2">
+        <f>(B124-$G$124)/$F$124</f>
+        <v>5.2339357429718882</v>
+      </c>
+      <c r="D124" s="2">
+        <v>4.4055</v>
+      </c>
+      <c r="E124" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F124">
+        <v>-0.996</v>
+      </c>
+      <c r="G124">
+        <v>9.6010000000000009</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A125" s="1">
+        <v>2</v>
+      </c>
+      <c r="B125" s="2">
+        <v>5.3159999999999998</v>
+      </c>
+      <c r="C125" s="2">
+        <f t="shared" ref="C125:C128" si="2">(B125-$G$124)/$F$124</f>
+        <v>4.3022088353413661</v>
+      </c>
+      <c r="D125" s="2">
+        <v>5.3319999999999999</v>
+      </c>
+      <c r="E125" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F125" s="17">
+        <v>-0.99344512309710387</v>
+      </c>
+      <c r="G125" s="18">
+        <v>9.6026888990426418</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A126" s="1">
+        <v>3</v>
+      </c>
+      <c r="B126" s="2">
+        <v>6.2439999999999998</v>
+      </c>
+      <c r="C126" s="2">
+        <f t="shared" si="2"/>
+        <v>3.3704819277108444</v>
+      </c>
+      <c r="D126" s="2">
+        <v>6.2525000000000004</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>4</v>
+      </c>
+      <c r="B127" s="2">
+        <v>7.7039999999999997</v>
+      </c>
+      <c r="C127" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9046184738955834</v>
+      </c>
+      <c r="D127" s="2">
+        <v>7.7093999999999996</v>
+      </c>
+      <c r="I127">
+        <v>9.6010000000000009</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A128" s="1">
+        <v>5</v>
+      </c>
+      <c r="B128" s="2">
+        <v>2.9289999999999998</v>
+      </c>
+      <c r="C128" s="2">
+        <f t="shared" si="2"/>
+        <v>6.6987951807228923</v>
+      </c>
+      <c r="D128" s="2">
+        <v>2.9449999999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130"/>
+      <c r="C130"/>
+      <c r="D130"/>
+      <c r="F130" s="13"/>
+    </row>
+    <row r="131" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B131"/>
+      <c r="C131"/>
+      <c r="D131"/>
+      <c r="F131" s="14"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A132" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B132" s="16"/>
+      <c r="C132"/>
+      <c r="D132" s="3">
+        <f>B124-D124</f>
+        <v>-1.7500000000000071E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A133" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B133" s="13">
+        <v>0.99999887397062648</v>
+      </c>
+      <c r="C133"/>
+      <c r="D133" s="3">
+        <f t="shared" ref="D133:D136" si="3">B125-D125</f>
+        <v>-1.6000000000000014E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A134" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B134" s="13">
+        <v>0.99999774794252083</v>
+      </c>
+      <c r="C134"/>
+      <c r="D134" s="3">
+        <f t="shared" si="3"/>
+        <v>-8.5000000000006182E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A135" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B135" s="13">
+        <v>0.99999699725669444</v>
+      </c>
+      <c r="C135"/>
+      <c r="D135" s="3">
+        <f t="shared" si="3"/>
+        <v>-5.3999999999998494E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A136" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B136" s="13">
+        <v>3.1305844469494228E-3</v>
+      </c>
+      <c r="C136"/>
+      <c r="D136" s="3">
+        <f t="shared" si="3"/>
+        <v>-1.6000000000000014E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A137" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B137" s="14">
+        <v>5</v>
+      </c>
+      <c r="C137"/>
+      <c r="D137"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B138"/>
+      <c r="C138"/>
+      <c r="D138"/>
+    </row>
+    <row r="139" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A139" t="s">
+        <v>25</v>
+      </c>
+      <c r="B139"/>
+      <c r="C139"/>
+      <c r="D139"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A140" s="15"/>
+      <c r="B140" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E140" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F140" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A141" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B141" s="13">
+        <v>1</v>
+      </c>
+      <c r="C141" s="13">
+        <v>13.055444186323061</v>
+      </c>
+      <c r="D141" s="13">
+        <v>13.055444186323061</v>
+      </c>
+      <c r="E141" s="13">
+        <v>1332112.2002995787</v>
+      </c>
+      <c r="F141" s="13">
+        <v>1.4343606539132147E-9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A142" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B142" s="13">
+        <v>3</v>
+      </c>
+      <c r="C142" s="13">
+        <v>2.9401676938444873E-5</v>
+      </c>
+      <c r="D142" s="13">
+        <v>9.8005589794816248E-6</v>
+      </c>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+    </row>
+    <row r="143" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A143" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" s="14">
+        <v>4</v>
+      </c>
+      <c r="C143" s="14">
+        <v>13.055473588</v>
+      </c>
+      <c r="D143" s="14"/>
+      <c r="E143" s="14"/>
+      <c r="F143" s="14"/>
+    </row>
+    <row r="144" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B144"/>
+      <c r="C144"/>
+      <c r="D144"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A145" s="15"/>
+      <c r="B145" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D145" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E145" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F145" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G145" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H145" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I145" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A146" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B146" s="13">
+        <v>9.6026888990426418</v>
+      </c>
+      <c r="C146" s="13">
+        <v>3.9587563043422726E-3</v>
+      </c>
+      <c r="D146" s="13">
+        <v>2425.6832602981053</v>
+      </c>
+      <c r="E146" s="13">
+        <v>1.5451413211730626E-10</v>
+      </c>
+      <c r="F146" s="13">
+        <v>9.5900903696683688</v>
+      </c>
+      <c r="G146" s="13">
+        <v>9.6152874284169148</v>
+      </c>
+      <c r="H146" s="13">
+        <v>9.5900903696683688</v>
+      </c>
+      <c r="I146" s="13">
+        <v>9.6152874284169148</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A147" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="14">
+        <v>-0.99344512309710387</v>
+      </c>
+      <c r="C147" s="14">
+        <v>8.6074295977919466E-4</v>
+      </c>
+      <c r="D147" s="14">
+        <v>-1154.1716511418822</v>
+      </c>
+      <c r="E147" s="14">
+        <v>1.4343606539132147E-9</v>
+      </c>
+      <c r="F147" s="14">
+        <v>-0.99618439134925207</v>
+      </c>
+      <c r="G147" s="14">
+        <v>-0.99070585484495566</v>
+      </c>
+      <c r="H147" s="14">
+        <v>-0.99618439134925207</v>
+      </c>
+      <c r="I147" s="14">
+        <v>-0.99070585484495566</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B148"/>
+      <c r="C148"/>
+      <c r="D148"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B149"/>
+      <c r="C149"/>
+      <c r="D149"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B150"/>
+      <c r="C150"/>
+      <c r="D150"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>